<commit_message>
Lectura de datos funcionando.
</commit_message>
<xml_diff>
--- a/plantillator/ndata/datos.xlsx
+++ b/plantillator/ndata/datos.xlsx
@@ -137,7 +137,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="642" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="643" uniqueCount="196">
   <si>
     <t>Valencia Sud 1</t>
   </si>
@@ -1267,7 +1267,7 @@
     </row>
     <row r="4" spans="1:6">
       <c r="B4" s="3" t="str">
-        <f>UPPER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(LOWER($C4)," ",""),"á","a"),"é","e"),"í","i"),"ó","o"),"ú","u"),"'",""),".",""))</f>
+        <f>UPPER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(LOWER($C4)," ",""),"á","a"),"é","e"),"í","i"),"ó","o"),"ú","u"),"'",""),".",""),"ñ","n"))</f>
         <v>VALENCIASUD1</v>
       </c>
       <c r="C4" s="3" t="s">
@@ -1280,7 +1280,7 @@
     </row>
     <row r="5" spans="1:6">
       <c r="B5" s="3" t="str">
-        <f>UPPER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(LOWER($C5)," ",""),"á","a"),"é","e"),"í","i"),"ó","o"),"ú","u"),"'",""),".",""))</f>
+        <f>UPPER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(LOWER($C5)," ",""),"á","a"),"é","e"),"í","i"),"ó","o"),"ú","u"),"'",""),".",""),"ñ","n"))</f>
         <v>VALENCIASUD2</v>
       </c>
       <c r="C5" s="3" t="s">
@@ -1328,7 +1328,7 @@
     </row>
     <row r="9" spans="1:6">
       <c r="B9" s="3" t="str">
-        <f t="shared" ref="B9:B14" si="0">UPPER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(LOWER($C9)," ",""),"á","a"),"é","e"),"í","i"),"ó","o"),"ú","u"),"'",""),".",""))</f>
+        <f t="shared" ref="B9:B14" si="0">UPPER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(LOWER($C9)," ",""),"á","a"),"é","e"),"í","i"),"ó","o"),"ú","u"),"'",""),".",""),"ñ","n"))</f>
         <v>AEROPUERTO</v>
       </c>
       <c r="C9" s="3" t="s">
@@ -1438,7 +1438,7 @@
     </row>
     <row r="18" spans="1:6">
       <c r="B18" s="3" t="str">
-        <f t="shared" ref="B18:B81" si="1">UPPER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(LOWER($C18)," ",""),"á","a"),"é","e"),"í","i"),"ó","o"),"ú","u"),"'",""),".",""))</f>
+        <f t="shared" ref="B18:B81" si="1">UPPER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(LOWER($C18)," ",""),"á","a"),"é","e"),"í","i"),"ó","o"),"ú","u"),"'",""),".",""),"ñ","n"))</f>
         <v>ROSAS</v>
       </c>
       <c r="C18" s="3" t="s">
@@ -1572,9 +1572,8 @@
       </c>
     </row>
     <row r="27" spans="1:6">
-      <c r="B27" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>PLAZAESPAÑA</v>
+      <c r="B27" s="3" t="s">
+        <v>128</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>50</v>
@@ -2398,7 +2397,7 @@
     </row>
     <row r="82" spans="2:6">
       <c r="B82" s="3" t="str">
-        <f t="shared" ref="B82:B87" si="2">UPPER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(LOWER($C82)," ",""),"á","a"),"é","e"),"í","i"),"ó","o"),"ú","u"),"'",""),".",""))</f>
+        <f t="shared" ref="B82:B87" si="2">UPPER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(LOWER($C82)," ",""),"á","a"),"é","e"),"í","i"),"ó","o"),"ú","u"),"'",""),".",""),"ñ","n"))</f>
         <v>TNARANJOS</v>
       </c>
       <c r="C82" s="3" t="s">

</xml_diff>